<commit_message>
Updates to BAU and alternate GDP, also carried through to FoPITY, EoSEUwGDPiR, and WebAppData
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\India InputData 5-6-2020\ctrl-settings\GDPGR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\20200527\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6511ADAF-042C-4405-A4CC-4A312EA12DD6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B501DB37-6045-4E8E-97BB-0F2C432FC625}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0B01EB80-3C2D-4F47-9BD5-4356DB1763F5}</author>
+  </authors>
+  <commentList>
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{0B01EB80-3C2D-4F47-9BD5-4356DB1763F5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Assumed to be as per official RBI counterfactual forecast</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
   <si>
     <t>About</t>
   </si>
@@ -203,9 +221,6 @@
     <t>World Bank</t>
   </si>
   <si>
-    <t>RBI</t>
-  </si>
-  <si>
     <t>Moody's</t>
   </si>
   <si>
@@ -216,9 +231,6 @@
 (Base Scenario)</t>
   </si>
   <si>
-    <t>Shrinkage</t>
-  </si>
-  <si>
     <t>World Bank - low</t>
   </si>
   <si>
@@ -243,12 +255,6 @@
     <t>https://www.cii.in/PublicationDetail.aspx?enc=zuvkFMUeRQ5DOr34VHgU+q2FCqvImS8h+0nQnlG8m5zQMi0OqNmYDbmu4OQt/zyXqsZaMZqaBOz17jO5kiK8beaL12OyxmfAhunCVE65HqgjLzXO2zFcwfMySBEKEXXZInWXyHg28Cg3wC9MTvYNtg==</t>
   </si>
   <si>
-    <t>Median Shrinkage</t>
-  </si>
-  <si>
-    <t>Avg. Shrinkage</t>
-  </si>
-  <si>
     <t>Median alternate GDP growth</t>
   </si>
   <si>
@@ -264,13 +270,6 @@
     <t>IMF to Fitch (columns B-F)</t>
   </si>
   <si>
-    <t>McKinsey
-(Scenario 2)</t>
-  </si>
-  <si>
-    <t>Pre- &amp; post-COVID GDP predictions - IMF, World Bank, RBI, Moody's, Fitch</t>
-  </si>
-  <si>
     <t>Compilation of estimates (via India Today)</t>
   </si>
   <si>
@@ -280,9 +279,6 @@
     <t>Infographic with pre- and post-COVID GDP projections</t>
   </si>
   <si>
-    <t>Scenario-based GDP impacts for India</t>
-  </si>
-  <si>
     <t>McKinsey &amp; Co.</t>
   </si>
   <si>
@@ -293,9 +289,6 @@
   </si>
   <si>
     <t>A plan for economic recovery</t>
-  </si>
-  <si>
-    <t>SARS-CoV-2 pandemic.  It uses the latest data available as of Apr 20,</t>
   </si>
   <si>
     <t>McKinsey (Scenario 2)</t>
@@ -318,16 +311,127 @@
     <t>Chart 1 &amp; Table 2, Pages 2-3 - GDP (Base scenario)</t>
   </si>
   <si>
-    <t>Scenario-based GDP predictions from Indian industry</t>
-  </si>
-  <si>
     <t>India Notes</t>
   </si>
   <si>
-    <t>Exhibit 1, Scenario 2</t>
-  </si>
-  <si>
-    <t>An average of estimates (as of 22/04/20) of COVID impacted GDP estimates for FY2021 is considered.</t>
+    <t>15th Finance 
+Commission</t>
+  </si>
+  <si>
+    <t>15th Finance Comm - low</t>
+  </si>
+  <si>
+    <t>15th Finance Comm - high</t>
+  </si>
+  <si>
+    <t>Goldman Sachs</t>
+  </si>
+  <si>
+    <t>https://www.livemint.com/news/india/indian-economy-may-contract-by-45-in-june-quarter-goldman-sachs-11589728732340.html</t>
+  </si>
+  <si>
+    <t>https://www.livemint.com/industry/banking/india-s-gdp-growth-in-2020-21-to-remain-in-negative-category-rbi-11590122207688.html</t>
+  </si>
+  <si>
+    <t>Crisil</t>
+  </si>
+  <si>
+    <t>https://www.crisil.com/en/home/our-analysis/reports/2020/05/minus-five.html</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2 pandemic.  It uses the latest data available as of May 2020,</t>
+  </si>
+  <si>
+    <t>Scenario-based GDP impacts for India (April 2020)</t>
+  </si>
+  <si>
+    <t>Goldman Sachs (via Livemint)</t>
+  </si>
+  <si>
+    <t>India’s GDP to shrink 45% in Q1FY21</t>
+  </si>
+  <si>
+    <t>15th Finance Commission of India (via Livemint)</t>
+  </si>
+  <si>
+    <t>India's GDP growth in 2020-21 to remain in negative territory: RBI</t>
+  </si>
+  <si>
+    <t>Projection 2, May 2020 - 15th Finance Commission of India</t>
+  </si>
+  <si>
+    <t>Projection 1, May 2020 - Goldman Sachs</t>
+  </si>
+  <si>
+    <t>Projection 3, May 2020 - Crisil</t>
+  </si>
+  <si>
+    <t>CRISIL Ratings</t>
+  </si>
+  <si>
+    <t>Minus Five</t>
+  </si>
+  <si>
+    <t>An average of projections (as of 27/05/20) of COVID impacted GDP for FY2021 is considered.</t>
+  </si>
+  <si>
+    <t>Pre- &amp; post-COVID GDP pojections - IMF, World Bank, RBI, Moody's, Fitch (April 2020)</t>
+  </si>
+  <si>
+    <t>Scenario-based GDP projections from Indian industry (April 2020)</t>
+  </si>
+  <si>
+    <t>Median reduction relative to 2019</t>
+  </si>
+  <si>
+    <t>Avg. Reduction</t>
+  </si>
+  <si>
+    <t>RBI*</t>
+  </si>
+  <si>
+    <t>As of 27 May 2020, the revised GDP forecast from RBI is yet to be published, based on a preliminary statement on the extent of GDP contraction expected.</t>
+  </si>
+  <si>
+    <t>Hence, it is not accounted for in the average.</t>
+  </si>
+  <si>
+    <t>15th Finance Commision of India + 
+RBI statement</t>
+  </si>
+  <si>
+    <t>McKinsey
+(Scenario 3)</t>
+  </si>
+  <si>
+    <t>Reduction</t>
+  </si>
+  <si>
+    <t>Exhibit 1, Scenario 3</t>
+  </si>
+  <si>
+    <t>min reductn</t>
+  </si>
+  <si>
+    <t>max reductn</t>
+  </si>
+  <si>
+    <t>Monetary Policy Report – April 2020</t>
+  </si>
+  <si>
+    <t>* The RBI forecast does not account for COVID impacts as it is based on a poll conducted prior to announcement of lockdown.</t>
+  </si>
+  <si>
+    <t>https://www.rbi.org.in/Scripts/PublicationsView.aspx?id=19439</t>
+  </si>
+  <si>
+    <t>Reserve Bank of India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RBI Professional forecasters poll </t>
+  </si>
+  <si>
+    <t>Table I.4</t>
   </si>
 </sst>
 </file>
@@ -338,7 +442,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,8 +514,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,6 +545,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,7 +584,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -485,9 +603,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -525,6 +640,18 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -548,16 +675,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>322</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>28897</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>296308</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>122740</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>324883</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>141790</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -580,7 +707,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7820347" y="571500"/>
+          <a:off x="9801547" y="590550"/>
           <a:ext cx="3953586" cy="2408740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -594,14 +721,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>121603</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>70346</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>55874</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>3670</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -624,8 +751,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="38100" y="3848100"/>
-          <a:ext cx="5747703" cy="5175746"/>
+          <a:off x="38100" y="3867149"/>
+          <a:ext cx="5599424" cy="5090021"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -637,14 +764,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>744714</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:colOff>249414</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>515177</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>229427</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -668,7 +795,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6688314" y="3829050"/>
+          <a:off x="5973939" y="3829050"/>
           <a:ext cx="5171138" cy="2876550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -682,13 +809,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>353047</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>160325</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -723,6 +850,12 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Deepthi Swamy" id="{A3B92C19-8074-40AA-AD9E-5E059CBE3A9D}" userId="0118328b9c39827d" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -986,18 +1119,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="G4" dT="2020-05-27T15:25:29.51" personId="{A3B92C19-8074-40AA-AD9E-5E059CBE3A9D}" id="{0B01EB80-3C2D-4F47-9BD5-4356DB1763F5}">
+    <text>Assumed to be as per official RBI counterfactual forecast</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A24:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="66.7109375" customWidth="1"/>
-    <col min="6" max="6" width="46" customWidth="1"/>
+    <col min="6" max="6" width="57.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1015,18 +1156,18 @@
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,265 +1180,358 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>81</v>
+        <v>95</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>43943</v>
       </c>
+      <c r="F13" s="9">
+        <v>43969</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>73</v>
+        <v>66</v>
+      </c>
+      <c r="F14" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="9">
+        <v>43973</v>
+      </c>
+      <c r="F20" s="9">
+        <v>43977</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="9">
+        <v>43930</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="D30" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="D19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D31" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="5"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>39</v>
+      <c r="A43" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>33</v>
-      </c>
+      <c r="A45" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="2"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B85" s="2"/>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="B97" s="2"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1306,271 +1540,412 @@
     <hyperlink ref="B8" r:id="rId1" xr:uid="{4E935FD4-3ED9-463A-899F-2DBCDD101C98}"/>
     <hyperlink ref="F8" r:id="rId2" xr:uid="{8B693CF3-2EFC-4813-A040-DA15351BD6A8}"/>
     <hyperlink ref="B15" r:id="rId3" xr:uid="{177EEAA9-CF54-488B-B469-F6CAB1C9DD47}"/>
+    <hyperlink ref="F15" r:id="rId4" xr:uid="{8B12342C-4ABA-4E37-95EE-9A8E74418D35}"/>
+    <hyperlink ref="B22" r:id="rId5" xr:uid="{4795503E-4388-46BC-9958-86ABCC5388AD}"/>
+    <hyperlink ref="F22" r:id="rId6" xr:uid="{29D9F7C1-1A9D-4550-836A-94A3AC0C73B0}"/>
+    <hyperlink ref="B28" r:id="rId7" xr:uid="{96610F8A-C938-4AD3-9C98-B7C498C19295}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E6303C-0F48-48BA-B94F-EBB8FB29306E}">
-  <dimension ref="A1:L17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E6303C-0F48-48BA-B94F-EBB8FB29306E}">
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D3" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F3" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="G3" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="H3" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" s="18">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="C3" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="D3" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="E3" s="18">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="F3" s="18">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="G3" s="17">
-        <f>D3</f>
-        <v>0.06</v>
-      </c>
-      <c r="H3" s="17">
-        <f>D3</f>
-        <v>0.06</v>
+      <c r="I3" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="K3" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="18">
+        <v>70</v>
+      </c>
+      <c r="B4" s="17">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="D4" s="32">
+        <v>0.06</v>
+      </c>
+      <c r="E4" s="17">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="F4" s="17">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="G4" s="16">
+        <v>0.06</v>
+      </c>
+      <c r="H4" s="16">
+        <f>G4</f>
+        <v>0.06</v>
+      </c>
+      <c r="I4" s="16">
+        <f t="shared" ref="I4:K4" si="0">H4</f>
+        <v>0.06</v>
+      </c>
+      <c r="J4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="K4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="17">
         <v>1.9E-2</v>
       </c>
-      <c r="C4" s="21">
-        <f>AVERAGE(B9:B10)</f>
+      <c r="C5" s="20">
+        <f>AVERAGE(B10:B11)</f>
         <v>2.75E-2</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D5" s="33">
         <v>5.5E-2</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E5" s="17">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F5" s="17">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G4" s="17">
-        <f>G3-G5</f>
-        <v>3.4999999999999996E-2</v>
-      </c>
-      <c r="H4" s="18">
+      <c r="G5" s="16">
+        <f>G4-G6</f>
+        <v>-0.03</v>
+      </c>
+      <c r="H5" s="17">
         <v>6.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="11">
-        <f>B3-B4</f>
+      <c r="I5" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="J5" s="17">
+        <f>AVERAGE(D10:D11)</f>
+        <v>-2.4999999999999998E-2</v>
+      </c>
+      <c r="K5" s="17">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="17">
+        <f>B4-B5</f>
         <v>3.9000000000000007E-2</v>
       </c>
-      <c r="C5" s="11">
-        <f t="shared" ref="C5:F5" si="0">C3-C4</f>
+      <c r="C6" s="17">
+        <f t="shared" ref="C6:F6" si="1">C4-C5</f>
         <v>2.2500000000000003E-2</v>
       </c>
-      <c r="D5" s="11">
-        <f t="shared" si="0"/>
+      <c r="D6" s="33">
+        <f t="shared" si="1"/>
         <v>4.9999999999999975E-3</v>
       </c>
-      <c r="E5" s="11">
-        <f t="shared" si="0"/>
+      <c r="E6" s="17">
+        <f t="shared" si="1"/>
         <v>2.8999999999999998E-2</v>
       </c>
-      <c r="F5" s="11">
-        <f t="shared" si="0"/>
+      <c r="F6" s="17">
+        <f t="shared" si="1"/>
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="G5" s="18">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H5" s="17">
-        <f>H3-H4</f>
+      <c r="G6" s="17">
+        <v>0.09</v>
+      </c>
+      <c r="H6" s="16">
+        <f>H4-H5</f>
         <v>5.3999999999999999E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="22">
-        <f>MEDIAN(B4:H4)</f>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="22">
-        <f>AVERAGE(B4:H4)</f>
-        <v>2.5071428571428574E-2</v>
-      </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="I6" s="16">
+        <f>I4-I5</f>
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="J6" s="16">
+        <f>J4-J5</f>
+        <v>8.4999999999999992E-2</v>
+      </c>
+      <c r="K6" s="16">
+        <f>K4-K5</f>
+        <v>0.11</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="22">
-        <f>MEDIAN(B5:H5)</f>
-        <v>2.8999999999999998E-2</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="22">
-        <f>AVERAGE(B5:H5)</f>
-        <v>3.1785714285714285E-2</v>
+      <c r="A7" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="21">
+        <f>MEDIAN(B5:C5,E5:K5)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="21">
+        <f>AVERAGE(B5:C5,E5:K5)</f>
+        <v>-1.0555555555555535E-3</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="22">
-        <f>MEDIAN(B3:H3)</f>
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="22">
-        <f>AVERAGE(B3:H3)</f>
-        <v>5.6857142857142863E-2</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="A8" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="21">
+        <f>MEDIAN(B6:B6:C6,E6:K6)</f>
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D8" s="21">
+        <f>AVERAGE(B6:C6,E6:K6)</f>
+        <v>5.8611111111111107E-2</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H8" s="34">
+        <f>MIN(B6:C6,E6:K6)</f>
+        <v>2.2500000000000003E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="20">
-        <v>1.4999999999999999E-2</v>
+      <c r="A9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="21">
+        <f>MEDIAN(B4:C4,E4:K4)</f>
+        <v>0.06</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="21">
+        <f>AVERAGE(B4:C4,E4:K4)</f>
+        <v>5.7555555555555554E-2</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="H9" s="34">
+        <f>MAX(B6:C6,E6:K6)</f>
+        <v>0.11</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="19">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="19">
+        <v>-0.06</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="19">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="C17" s="27"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="29" t="s">
+      <c r="B18" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="28"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="C18" s="27"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B19" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="28"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="28"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>76</v>
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="28"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="27"/>
+      <c r="B23" s="28"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1" xr:uid="{F1A24B7E-C1F6-4E4E-BAB4-16D5AF9FD11D}"/>
-    <hyperlink ref="B14" r:id="rId2" xr:uid="{E89F511E-8399-4A1A-93DB-920BF96CB1D1}"/>
-    <hyperlink ref="B15" r:id="rId3" xr:uid="{6BF9F150-CB6E-414F-A71A-FE1A0E6C36EA}"/>
+    <hyperlink ref="B17" r:id="rId1" xr:uid="{F1A24B7E-C1F6-4E4E-BAB4-16D5AF9FD11D}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{E89F511E-8399-4A1A-93DB-920BF96CB1D1}"/>
+    <hyperlink ref="B19" r:id="rId3" xr:uid="{6BF9F150-CB6E-414F-A71A-FE1A0E6C36EA}"/>
+    <hyperlink ref="B20" r:id="rId4" xr:uid="{DF501DC0-5A03-4C1D-969F-5D0E6F714519}"/>
+    <hyperlink ref="B21" r:id="rId5" xr:uid="{A241EAC3-FD54-4560-ABF2-C08155C71F85}"/>
+    <hyperlink ref="B22" r:id="rId6" xr:uid="{56E9BC92-0147-48B8-9CF3-3C8A9D988885}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+  <drawing r:id="rId8"/>
+  <legacyDrawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -1602,9 +1977,9 @@
       <c r="A2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="23">
-        <f>'India Data'!D6</f>
-        <v>2.5071428571428574E-2</v>
+      <c r="B2" s="22">
+        <f>'India Data'!D7</f>
+        <v>-1.0555555555555535E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1640,9 +2015,9 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="23">
-        <f>'India Data'!D8</f>
-        <v>5.6857142857142863E-2</v>
+      <c r="B2" s="22">
+        <f>'India Data'!D9</f>
+        <v>5.7555555555555554E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ensure GDPGR values are clean multiples of slider interval
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\20200527\GDPGR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\ctrl-settings\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B501DB37-6045-4E8E-97BB-0F2C432FC625}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
     <sheet name="GDPGR-alternate" sheetId="2" r:id="rId3"/>
     <sheet name="GDPGR-bau" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,17 +33,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={0B01EB80-3C2D-4F47-9BD5-4356DB1763F5}</author>
   </authors>
   <commentList>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{0B01EB80-3C2D-4F47-9BD5-4356DB1763F5}">
+    <comment ref="G4" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Assumed to be as per official RBI counterfactual forecast</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -437,7 +445,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -1128,30 +1136,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A25" sqref="A24:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="66.7109375" customWidth="1"/>
-    <col min="6" max="6" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="66.73046875" customWidth="1"/>
+    <col min="6" max="6" width="57.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1162,7 +1170,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>60</v>
       </c>
@@ -1170,7 +1178,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B6" s="9">
         <v>43945</v>
       </c>
@@ -1178,7 +1186,7 @@
         <v>43930</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>61</v>
       </c>
@@ -1186,7 +1194,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>50</v>
       </c>
@@ -1194,7 +1202,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>62</v>
       </c>
@@ -1202,7 +1210,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
         <v>95</v>
       </c>
@@ -1210,7 +1218,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>65</v>
       </c>
@@ -1218,7 +1226,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B13" s="9">
         <v>43943</v>
       </c>
@@ -1226,7 +1234,7 @@
         <v>43969</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>66</v>
       </c>
@@ -1234,7 +1242,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B15" s="3" t="s">
         <v>54</v>
       </c>
@@ -1242,12 +1250,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
         <v>88</v>
       </c>
@@ -1255,7 +1263,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>86</v>
       </c>
@@ -1263,7 +1271,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B20" s="9">
         <v>43973</v>
       </c>
@@ -1271,7 +1279,7 @@
         <v>43977</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>87</v>
       </c>
@@ -1279,7 +1287,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
         <v>79</v>
       </c>
@@ -1287,45 +1295,45 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>110</v>
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B26" s="9">
         <v>43930</v>
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>107</v>
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1342,7 @@
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1342,208 +1350,208 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B55" s="5"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B97" s="2"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{4E935FD4-3ED9-463A-899F-2DBCDD101C98}"/>
-    <hyperlink ref="F8" r:id="rId2" xr:uid="{8B693CF3-2EFC-4813-A040-DA15351BD6A8}"/>
-    <hyperlink ref="B15" r:id="rId3" xr:uid="{177EEAA9-CF54-488B-B469-F6CAB1C9DD47}"/>
-    <hyperlink ref="F15" r:id="rId4" xr:uid="{8B12342C-4ABA-4E37-95EE-9A8E74418D35}"/>
-    <hyperlink ref="B22" r:id="rId5" xr:uid="{4795503E-4388-46BC-9958-86ABCC5388AD}"/>
-    <hyperlink ref="F22" r:id="rId6" xr:uid="{29D9F7C1-1A9D-4550-836A-94A3AC0C73B0}"/>
-    <hyperlink ref="B28" r:id="rId7" xr:uid="{96610F8A-C938-4AD3-9C98-B7C498C19295}"/>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="B15" r:id="rId3"/>
+    <hyperlink ref="F15" r:id="rId4"/>
+    <hyperlink ref="B22" r:id="rId5"/>
+    <hyperlink ref="F22" r:id="rId6"/>
+    <hyperlink ref="B28" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>
@@ -1551,35 +1559,35 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06E6303C-0F48-48BA-B94F-EBB8FB29306E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.59765625" customWidth="1"/>
+    <col min="3" max="3" width="24.73046875" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" s="4"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="24"/>
       <c r="B3" s="25" t="s">
         <v>42</v>
@@ -1615,7 +1623,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
         <v>70</v>
       </c>
@@ -1654,7 +1662,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
         <v>71</v>
       </c>
@@ -1692,7 +1700,7 @@
         <v>-0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>103</v>
       </c>
@@ -1736,7 +1744,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
         <v>55</v>
       </c>
@@ -1756,7 +1764,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
         <v>96</v>
       </c>
@@ -1781,7 +1789,7 @@
         <v>2.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
         <v>57</v>
       </c>
@@ -1806,7 +1814,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -1822,7 +1830,7 @@
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -1838,38 +1846,38 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="31" t="s">
         <v>108</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="31" t="s">
         <v>99</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="31" t="s">
         <v>100</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="29"/>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="27" t="s">
         <v>59</v>
       </c>
@@ -1878,7 +1886,7 @@
       </c>
       <c r="C17" s="27"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="27" t="s">
         <v>51</v>
       </c>
@@ -1887,7 +1895,7 @@
       </c>
       <c r="C18" s="27"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="27" t="s">
         <v>53</v>
       </c>
@@ -1896,7 +1904,7 @@
       </c>
       <c r="C19" s="27"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>77</v>
       </c>
@@ -1904,7 +1912,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="24" x14ac:dyDescent="0.45">
       <c r="A21" s="30" t="s">
         <v>101</v>
       </c>
@@ -1913,7 +1921,7 @@
       </c>
       <c r="C21" s="28"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="27" t="s">
         <v>80</v>
       </c>
@@ -1921,11 +1929,11 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="27"/>
       <c r="B23" s="28"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B24" s="23" t="s">
         <v>67</v>
       </c>
@@ -1935,12 +1943,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" xr:uid="{F1A24B7E-C1F6-4E4E-BAB4-16D5AF9FD11D}"/>
-    <hyperlink ref="B18" r:id="rId2" xr:uid="{E89F511E-8399-4A1A-93DB-920BF96CB1D1}"/>
-    <hyperlink ref="B19" r:id="rId3" xr:uid="{6BF9F150-CB6E-414F-A71A-FE1A0E6C36EA}"/>
-    <hyperlink ref="B20" r:id="rId4" xr:uid="{DF501DC0-5A03-4C1D-969F-5D0E6F714519}"/>
-    <hyperlink ref="B21" r:id="rId5" xr:uid="{A241EAC3-FD54-4560-ABF2-C08155C71F85}"/>
-    <hyperlink ref="B22" r:id="rId6" xr:uid="{56E9BC92-0147-48B8-9CF3-3C8A9D988885}"/>
+    <hyperlink ref="B17" r:id="rId1"/>
+    <hyperlink ref="B18" r:id="rId2"/>
+    <hyperlink ref="B19" r:id="rId3"/>
+    <hyperlink ref="B20" r:id="rId4"/>
+    <hyperlink ref="B21" r:id="rId5"/>
+    <hyperlink ref="B22" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -1950,22 +1958,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
@@ -1973,13 +1981,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="22">
-        <f>'India Data'!D7</f>
-        <v>-1.0555555555555535E-3</v>
+        <f>ROUND('India Data'!D7,3)</f>
+        <v>-1E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1988,22 +1996,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAE059C-14EE-421B-BDC1-8D6581F6B587}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
@@ -2011,13 +2019,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="22">
-        <f>'India Data'!D9</f>
-        <v>5.7555555555555554E-2</v>
+        <f>ROUND('India Data'!D9,3)</f>
+        <v>5.8000000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed rounding adjustment from GDPGR
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -17,7 +17,7 @@
     <sheet name="GDPGR-alternate" sheetId="2" r:id="rId3"/>
     <sheet name="GDPGR-bau" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1965,7 +1965,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1986,8 +1986,8 @@
         <v>26</v>
       </c>
       <c r="B2" s="22">
-        <f>ROUND('India Data'!D7,3)</f>
-        <v>-1E-3</v>
+        <f>'India Data'!D7</f>
+        <v>-1.0555555555555535E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2024,8 +2024,8 @@
         <v>28</v>
       </c>
       <c r="B2" s="22">
-        <f>ROUND('India Data'!D9,3)</f>
-        <v>5.8000000000000003E-2</v>
+        <f>'India Data'!D9</f>
+        <v>5.7555555555555554E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update COVID-19 recession settings
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
+++ b/InputData/ctrl-settings/GDPGR/GDP Growth Rates.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-india\InputData\ctrl-settings\GDPGR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-india\InputData\ctrl-settings\GDPGR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5445"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="India Data" sheetId="3" r:id="rId2"/>
-    <sheet name="GDPGR-alternate" sheetId="2" r:id="rId3"/>
-    <sheet name="GDPGR-bau" sheetId="8" r:id="rId4"/>
+    <sheet name="India Data-May 2020" sheetId="3" r:id="rId2"/>
+    <sheet name="India Data-Jan 2021" sheetId="9" r:id="rId3"/>
+    <sheet name="GDPGR-alternate" sheetId="2" r:id="rId4"/>
+    <sheet name="GDPGR-bau" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="119">
   <si>
     <t>About</t>
   </si>
@@ -263,9 +266,6 @@
     <t>https://www.cii.in/PublicationDetail.aspx?enc=zuvkFMUeRQ5DOr34VHgU+q2FCqvImS8h+0nQnlG8m5zQMi0OqNmYDbmu4OQt/zyXqsZaMZqaBOz17jO5kiK8beaL12OyxmfAhunCVE65HqgjLzXO2zFcwfMySBEKEXXZInWXyHg28Cg3wC9MTvYNtg==</t>
   </si>
   <si>
-    <t>Median alternate GDP growth</t>
-  </si>
-  <si>
     <t>Avg. Alt GDP</t>
   </si>
   <si>
@@ -303,9 +303,6 @@
   </si>
   <si>
     <t>CII (Base Scenario)</t>
-  </si>
-  <si>
-    <t>India - BAU and Alternate GDP projections for Financial Year 2020</t>
   </si>
   <si>
     <t>Pre-COVID forecast
@@ -380,9 +377,6 @@
     <t>Minus Five</t>
   </si>
   <si>
-    <t>An average of projections (as of 27/05/20) of COVID impacted GDP for FY2021 is considered.</t>
-  </si>
-  <si>
     <t>Pre- &amp; post-COVID GDP pojections - IMF, World Bank, RBI, Moody's, Fitch (April 2020)</t>
   </si>
   <si>
@@ -418,12 +412,6 @@
     <t>Exhibit 1, Scenario 3</t>
   </si>
   <si>
-    <t>min reductn</t>
-  </si>
-  <si>
-    <t>max reductn</t>
-  </si>
-  <si>
     <t>Monetary Policy Report – April 2020</t>
   </si>
   <si>
@@ -440,6 +428,39 @@
   </si>
   <si>
     <t>Table I.4</t>
+  </si>
+  <si>
+    <t>India - BAU and Alternate GDP projections for Financial Year 2020-21</t>
+  </si>
+  <si>
+    <t>Alternate GDP Projection, Jan 2021 - NSO</t>
+  </si>
+  <si>
+    <t>National Statistical Office (NSO) via Indian Express</t>
+  </si>
+  <si>
+    <t>India’s GDP to contract 7.7% in current fiscal, advance estimates show</t>
+  </si>
+  <si>
+    <t>https://indianexpress.com/article/business/economy/gdp-to-contract-7-7-in-current-fiscal-advance-estimates-show-7137643/</t>
+  </si>
+  <si>
+    <t>(as per National Statistical Office)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As of Jan 2021, India's GDP is estimated to contract </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> in FY2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Median alternate GDP growth </t>
+  </si>
+  <si>
+    <t>For alternate GDP, a more recent official estimate (as of Jan 2021) is considered.</t>
+  </si>
+  <si>
+    <t>For counter-factual BAU GDP for FY2021, an average of projections (as of May 2020) is considered.</t>
   </si>
 </sst>
 </file>
@@ -592,7 +613,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -660,6 +681,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1139,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A24:A25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1164,18 +1189,18 @@
         <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1188,10 +1213,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -1204,26 +1229,26 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
@@ -1236,10 +1261,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -1247,28 +1272,28 @@
         <v>54</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -1281,18 +1306,18 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -1301,36 +1326,47 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B24" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" t="s">
         <v>110</v>
       </c>
-      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B26" s="9">
         <v>43930</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="F26" s="9">
+        <v>44204</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B28" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -1338,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E30" s="1"/>
     </row>
@@ -1347,13 +1383,16 @@
         <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>1</v>
       </c>
+      <c r="D32" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
@@ -1418,7 +1457,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
@@ -1562,8 +1601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1577,7 +1616,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>108</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1596,7 +1635,7 @@
         <v>43</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>44</v>
@@ -1605,27 +1644,27 @@
         <v>45</v>
       </c>
       <c r="G3" s="26" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H3" s="26" t="s">
         <v>46</v>
       </c>
       <c r="I3" s="26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J3" s="26" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="L3" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B4" s="17">
         <v>5.8000000000000003E-2</v>
@@ -1664,7 +1703,7 @@
     </row>
     <row r="5" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B5" s="17">
         <v>1.9E-2</v>
@@ -1702,7 +1741,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B6" s="17">
         <f>B4-B5</f>
@@ -1746,14 +1785,14 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="12" t="s">
-        <v>55</v>
+        <v>116</v>
       </c>
       <c r="B7" s="21">
         <f>MEDIAN(B5:C5,E5:K5)</f>
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="21">
         <f>AVERAGE(B5:C5,E5:K5)</f>
@@ -1766,14 +1805,14 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="12" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B8" s="21">
         <f>MEDIAN(B6:B6:C6,E6:K6)</f>
         <v>4.9999999999999996E-2</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D8" s="21">
         <f>AVERAGE(B6:C6,E6:K6)</f>
@@ -1781,38 +1820,27 @@
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="14"/>
-      <c r="G8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H8" s="34">
-        <f>MIN(B6:C6,E6:K6)</f>
-        <v>2.2500000000000003E-2</v>
-      </c>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="21">
         <f>MEDIAN(B4:C4,E4:K4)</f>
         <v>0.06</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="21">
+        <v>57</v>
+      </c>
+      <c r="D9" s="35">
         <f>AVERAGE(B4:C4,E4:K4)</f>
         <v>5.7555555555555554E-2</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" s="34">
-        <f>MAX(B6:C6,E6:K6)</f>
-        <v>0.11</v>
-      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="34"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
@@ -1822,7 +1850,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D10" s="19">
         <v>-0.06</v>
@@ -1838,7 +1866,7 @@
         <v>0.04</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="18">
         <v>0.01</v>
@@ -1848,21 +1876,21 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="19"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="31" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="19"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="31" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -1879,7 +1907,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>50</v>
@@ -1906,27 +1934,27 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="24" x14ac:dyDescent="0.45">
       <c r="A21" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="28" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C21" s="28"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B22" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -1935,10 +1963,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B24" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="23" t="s">
         <v>67</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1959,39 +1987,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="8" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="30.59765625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="36">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="22">
-        <f>'India Data'!D7</f>
-        <v>-1.0555555555555535E-3</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2003,7 +2030,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2021,10 +2048,48 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="22">
+        <f>-'India Data-Jan 2021'!F1</f>
+        <v>-7.6999999999999999E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="22">
-        <f>'India Data'!D9</f>
+        <f>'India Data-May 2020'!D9</f>
         <v>5.7555555555555554E-2</v>
       </c>
     </row>

</xml_diff>